<commit_message>
4 e 5 completo
</commit_message>
<xml_diff>
--- a/StockingProblemProject/Testes/Problema3/testes_tamanho_torneio/statistic_average_fitness_avaliado.xlsx
+++ b/StockingProblemProject/Testes/Problema3/testes_tamanho_torneio/statistic_average_fitness_avaliado.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna Leitão\Desktop\Escola\IA\IAProject_StockingProblem\StockingProblemProject\Testes\Problema3\testes_tamanho_torneio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75630C3B-25F2-40C7-9C41-6928F84CC7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB776861-BCA1-41B7-AADF-4A63BDEEB90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="10212" windowHeight="9264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3statistic_average_fitness_aval" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1824,7 +1824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>